<commit_message>
cambios en el modelado de la óptica
</commit_message>
<xml_diff>
--- a/HT-5/Optica BAC-03-Ficha tecnica de un canal.xlsx
+++ b/HT-5/Optica BAC-03-Ficha tecnica de un canal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A93CA4-A7D8-D84A-BADF-954F5817932D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F11C73-3B87-1747-A370-38A7B5DD959E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5900" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="28800" yWindow="-5900" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-03-1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="BAC-03-3" sheetId="8" r:id="rId3"/>
     <sheet name="BAC-03-4" sheetId="9" r:id="rId4"/>
     <sheet name="BAC-03-5" sheetId="10" r:id="rId5"/>
-    <sheet name="BAC-03-6" sheetId="11" r:id="rId6"/>
-    <sheet name="BAC-03-7" sheetId="13" r:id="rId7"/>
-    <sheet name="BAC-03-8" sheetId="14" r:id="rId8"/>
-    <sheet name="BAC-03-10" sheetId="15" r:id="rId9"/>
+    <sheet name="BAC-03-5 (2)" sheetId="16" r:id="rId6"/>
+    <sheet name="BAC-03-6" sheetId="11" r:id="rId7"/>
+    <sheet name="BAC-03-7" sheetId="13" r:id="rId8"/>
+    <sheet name="BAC-03-8" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -119,27 +119,9 @@
     <t>A2</t>
   </si>
   <si>
-    <t>Aprovisionamiento de monturas</t>
-  </si>
-  <si>
     <t>Aprovisionamiento</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>Aplicación de fórmula</t>
-  </si>
-  <si>
-    <t>Transformación</t>
-  </si>
-  <si>
-    <t>Defiinir el tipo de corte que se la hará al lente</t>
-  </si>
-  <si>
-    <t>Pulir el lente</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
@@ -224,16 +206,28 @@
     <t xml:space="preserve">Manejar devoluciones, reclamos y procesos de aseguramiento de calidad con los proveedores </t>
   </si>
   <si>
-    <t>Cortar el lente de acuerdo con la montura definida</t>
-  </si>
-  <si>
-    <t>Revisar la fórmula o las modificaciones a aplicar</t>
-  </si>
-  <si>
-    <t>Empleado laboratorio</t>
-  </si>
-  <si>
     <t>Aprovisioinamiento de lentes</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Entrega y distribución de monturas</t>
+  </si>
+  <si>
+    <t>Desempacar y mostrar los productos en los estantes</t>
+  </si>
+  <si>
+    <t>Entregarle las monturas junto con las fórmulas para su respectiva modificación</t>
+  </si>
+  <si>
+    <t>Recibir las monturas junto con su respectiva modificación de fórmula de lentes</t>
+  </si>
+  <si>
+    <t>Manejar devoluciones en caso de que las gafas no cumplan con la calidad requerida tanto del cliente como de la Óptica</t>
+  </si>
+  <si>
+    <t>Modificación de las monturas</t>
   </si>
 </sst>
 </file>
@@ -330,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -346,9 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -363,10 +354,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +671,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -755,17 +742,17 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -773,58 +760,58 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.15">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>3</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="B12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -837,7 +824,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -909,17 +896,17 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.15">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.15">
@@ -927,26 +914,26 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1037,13 +1024,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -1051,13 +1038,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -1065,26 +1052,26 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1138,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1172,13 +1159,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.15">
@@ -1186,32 +1173,32 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1299,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
@@ -1313,32 +1300,32 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1347,6 +1334,119 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC23699-5522-D349-A5C8-F5BF9DDF1F2E}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0CEC55-42F1-4C9D-94B6-0A3DC2619C0F}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1392,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1426,64 +1526,64 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1491,12 +1591,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD743F-5732-48A8-9B15-61A983AA847C}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1537,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1571,13 +1671,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.15">
@@ -1585,13 +1685,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1600,12 +1700,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01BD858-72F0-4803-BCED-49D604DC8C85}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="A10:D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1646,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1655,7 +1755,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1675,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -1683,13 +1783,13 @@
         <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -1697,147 +1797,24 @@
         <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F2B678-6A08-4DCD-A7B0-10E20E2DA48D}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="4" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.15">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>